<commit_message>
Pushing everything else 2
</commit_message>
<xml_diff>
--- a/CS444_Fall20_homework_grade.xlsx
+++ b/CS444_Fall20_homework_grade.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Comments on HW</t>
   </si>
@@ -39,6 +39,18 @@
   </si>
   <si>
     <t>testio_mod-dotadan.script missing debug_log; remotegdb script OK</t>
+  </si>
+  <si>
+    <t>hw1_part2</t>
+  </si>
+  <si>
+    <t>script looks OK</t>
+  </si>
+  <si>
+    <t>hw2</t>
+  </si>
+  <si>
+    <t>script looks OK, code in ulib.s OK</t>
   </si>
 </sst>
 </file>
@@ -82,14 +94,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -371,10 +386,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection sqref="A1:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -391,7 +406,7 @@
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
     </row>
@@ -402,8 +417,30 @@
       <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="4">
         <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="4">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>